<commit_message>
Updating local_settings_template for new data, and including FFM data for loading
</commit_message>
<xml_diff>
--- a/data/base/Sierra_site_FFM_preds-1.xlsx
+++ b/data/base/Sierra_site_FFM_preds-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20349"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20350"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsx\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsx\Dropbox\Code\belleflopt\data\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCFD2E4C-63C6-4B32-BF24-88770C771D47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62600FDB-7229-4006-B7A1-A7E580CDE4FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15360" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sierra_FFM_preds" sheetId="1" r:id="rId1"/>
@@ -18177,16 +18177,16 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -18224,7 +18224,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -18259,7 +18259,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -18295,7 +18295,7 @@
       </c>
       <c r="L3" s="9"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -18333,7 +18333,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -18369,7 +18369,7 @@
       </c>
       <c r="L5" s="9"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -18405,7 +18405,7 @@
       </c>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -18441,7 +18441,7 @@
       </c>
       <c r="L7" s="9"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -18477,7 +18477,7 @@
       </c>
       <c r="L8" s="9"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -18515,7 +18515,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -18553,7 +18553,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -18591,7 +18591,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -18627,7 +18627,7 @@
       </c>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -18663,7 +18663,7 @@
       </c>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -18701,7 +18701,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -18737,7 +18737,7 @@
       </c>
       <c r="L15" s="9"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -18773,7 +18773,7 @@
       </c>
       <c r="L16" s="9"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -18811,7 +18811,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -18847,7 +18847,7 @@
       </c>
       <c r="L18" s="9"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -18883,7 +18883,7 @@
       </c>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -18919,7 +18919,7 @@
       </c>
       <c r="L20" s="9"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -18955,7 +18955,7 @@
       </c>
       <c r="L21" s="9"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -18993,7 +18993,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -19029,7 +19029,7 @@
       </c>
       <c r="L23" s="9"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -19067,7 +19067,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -19103,7 +19103,7 @@
       </c>
       <c r="L25" s="9"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>8</v>
       </c>
@@ -19135,7 +19135,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>10</v>
       </c>
@@ -19167,7 +19167,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>11</v>
       </c>
@@ -19202,7 +19202,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -19234,7 +19234,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>13</v>
       </c>
@@ -19266,7 +19266,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>15</v>
       </c>
@@ -19298,7 +19298,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>16</v>
       </c>
@@ -19330,7 +19330,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>17</v>
       </c>
@@ -19365,7 +19365,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>18</v>
       </c>
@@ -19400,7 +19400,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>19</v>
       </c>
@@ -19435,7 +19435,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>20</v>
       </c>
@@ -19467,7 +19467,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>21</v>
       </c>
@@ -19499,7 +19499,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>22</v>
       </c>
@@ -19534,7 +19534,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>23</v>
       </c>
@@ -19566,7 +19566,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>24</v>
       </c>
@@ -19598,7 +19598,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>25</v>
       </c>
@@ -19633,7 +19633,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>26</v>
       </c>
@@ -19665,7 +19665,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>27</v>
       </c>
@@ -19697,7 +19697,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>28</v>
       </c>
@@ -19729,7 +19729,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>29</v>
       </c>
@@ -19761,7 +19761,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>30</v>
       </c>
@@ -19796,7 +19796,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>31</v>
       </c>
@@ -19828,7 +19828,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>32</v>
       </c>
@@ -19863,7 +19863,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>33</v>
       </c>
@@ -19910,17 +19910,17 @@
       <selection pane="topRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.44140625" customWidth="1"/>
-    <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -19973,7 +19973,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -20029,7 +20029,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -20086,7 +20086,7 @@
       </c>
       <c r="T3" s="9"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -20130,7 +20130,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -20187,7 +20187,7 @@
       </c>
       <c r="T5" s="9"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -20244,7 +20244,7 @@
       </c>
       <c r="T6" s="9"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -20301,7 +20301,7 @@
       </c>
       <c r="T7" s="9"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -20358,7 +20358,7 @@
       </c>
       <c r="T8" s="9"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -20402,7 +20402,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -20446,7 +20446,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -20490,7 +20490,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -20547,7 +20547,7 @@
       </c>
       <c r="T12" s="9"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -20604,7 +20604,7 @@
       </c>
       <c r="T13" s="9"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -20648,7 +20648,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -20705,7 +20705,7 @@
       </c>
       <c r="T15" s="9"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -20762,7 +20762,7 @@
       </c>
       <c r="T16" s="9"/>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -20806,7 +20806,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -20863,7 +20863,7 @@
       </c>
       <c r="T18" s="9"/>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -20920,7 +20920,7 @@
       </c>
       <c r="T19" s="9"/>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -20977,7 +20977,7 @@
       </c>
       <c r="T20" s="9"/>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -21034,7 +21034,7 @@
       </c>
       <c r="T21" s="9"/>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -21078,7 +21078,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -21135,7 +21135,7 @@
       </c>
       <c r="T23" s="9"/>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -21179,7 +21179,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -21236,7 +21236,7 @@
       </c>
       <c r="T25" s="9"/>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>2</v>
       </c>
@@ -21382,7 +21382,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
         <v>8</v>
       </c>
@@ -21480,7 +21480,7 @@
       </c>
       <c r="AW30" s="11"/>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>39</v>
       </c>
@@ -21626,7 +21626,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -21823,7 +21823,7 @@
         <v>12.4</v>
       </c>
     </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -22020,7 +22020,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="34" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -22217,7 +22217,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="35" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -22414,7 +22414,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="36" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -22611,11 +22611,11 @@
         <v>352.8</v>
       </c>
     </row>
-    <row r="37" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AL37" s="5"/>
       <c r="AM37" s="5"/>
     </row>
-    <row r="38" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -22812,7 +22812,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="39" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -23009,7 +23009,7 @@
         <v>281.5</v>
       </c>
     </row>
-    <row r="40" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -23206,7 +23206,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>37</v>
       </c>
@@ -23403,7 +23403,7 @@
         <v>15.800000000000011</v>
       </c>
     </row>
-    <row r="42" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -23600,10 +23600,10 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
     </row>
-    <row r="46" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
@@ -23623,10 +23623,10 @@
       <c r="X46" s="1"/>
       <c r="Y46" s="1"/>
     </row>
-    <row r="47" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
     </row>
-    <row r="48" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>2</v>
       </c>
@@ -23648,7 +23648,7 @@
       <c r="X48" s="2"/>
       <c r="Y48" s="2"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>3</v>
       </c>
@@ -23670,7 +23670,7 @@
       <c r="X49" s="2"/>
       <c r="Y49" s="2"/>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>4</v>
       </c>
@@ -23692,7 +23692,7 @@
       <c r="X50" s="2"/>
       <c r="Y50" s="2"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>5</v>
       </c>
@@ -23714,7 +23714,7 @@
       <c r="X51" s="2"/>
       <c r="Y51" s="2"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>6</v>
       </c>
@@ -23736,10 +23736,10 @@
       <c r="X52" s="2"/>
       <c r="Y52" s="2"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>34</v>
       </c>
@@ -23761,7 +23761,7 @@
       <c r="X54" s="2"/>
       <c r="Y54" s="2"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>35</v>
       </c>
@@ -23783,7 +23783,7 @@
       <c r="X55" s="2"/>
       <c r="Y55" s="2"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>36</v>
       </c>
@@ -23805,7 +23805,7 @@
       <c r="X56" s="2"/>
       <c r="Y56" s="2"/>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>37</v>
       </c>
@@ -23827,7 +23827,7 @@
       <c r="X57" s="2"/>
       <c r="Y57" s="2"/>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>38</v>
       </c>
@@ -23849,17 +23849,29 @@
       <c r="X58" s="2"/>
       <c r="Y58" s="2"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="AV30:AW30"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="AB30:AC30"/>
+    <mergeCell ref="AD30:AE30"/>
+    <mergeCell ref="AF30:AG30"/>
+    <mergeCell ref="AH30:AI30"/>
+    <mergeCell ref="AJ30:AK30"/>
+    <mergeCell ref="AL30:AM30"/>
+    <mergeCell ref="AN30:AO30"/>
+    <mergeCell ref="AP30:AQ30"/>
+    <mergeCell ref="AR30:AS30"/>
+    <mergeCell ref="AT30:AU30"/>
     <mergeCell ref="X30:Y30"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="D30:E30"/>
@@ -23872,18 +23884,6 @@
     <mergeCell ref="R30:S30"/>
     <mergeCell ref="T30:U30"/>
     <mergeCell ref="V30:W30"/>
-    <mergeCell ref="AV30:AW30"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="AB30:AC30"/>
-    <mergeCell ref="AD30:AE30"/>
-    <mergeCell ref="AF30:AG30"/>
-    <mergeCell ref="AH30:AI30"/>
-    <mergeCell ref="AJ30:AK30"/>
-    <mergeCell ref="AL30:AM30"/>
-    <mergeCell ref="AN30:AO30"/>
-    <mergeCell ref="AP30:AQ30"/>
-    <mergeCell ref="AR30:AS30"/>
-    <mergeCell ref="AT30:AU30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -23900,17 +23900,17 @@
       <selection pane="topRight" activeCell="Y80" sqref="Y80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.44140625" customWidth="1"/>
-    <col min="12" max="12" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -23963,7 +23963,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -24019,7 +24019,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -24076,7 +24076,7 @@
       </c>
       <c r="T3" s="9"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -24120,7 +24120,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -24177,7 +24177,7 @@
       </c>
       <c r="T5" s="9"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -24234,7 +24234,7 @@
       </c>
       <c r="T6" s="9"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -24291,7 +24291,7 @@
       </c>
       <c r="T7" s="9"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -24348,7 +24348,7 @@
       </c>
       <c r="T8" s="9"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -24392,7 +24392,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -24436,7 +24436,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -24480,7 +24480,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -24537,7 +24537,7 @@
       </c>
       <c r="T12" s="9"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -24594,7 +24594,7 @@
       </c>
       <c r="T13" s="9"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -24638,7 +24638,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -24695,7 +24695,7 @@
       </c>
       <c r="T15" s="9"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -24752,7 +24752,7 @@
       </c>
       <c r="T16" s="9"/>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -24796,7 +24796,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -24853,7 +24853,7 @@
       </c>
       <c r="T18" s="9"/>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -24910,7 +24910,7 @@
       </c>
       <c r="T19" s="9"/>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -24967,7 +24967,7 @@
       </c>
       <c r="T20" s="9"/>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -25024,7 +25024,7 @@
       </c>
       <c r="T21" s="9"/>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -25068,7 +25068,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -25125,7 +25125,7 @@
       </c>
       <c r="T23" s="9"/>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -25169,7 +25169,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -25226,7 +25226,7 @@
       </c>
       <c r="T25" s="9"/>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B29" s="10">
         <v>2</v>
       </c>
@@ -25372,7 +25372,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
         <v>8</v>
       </c>
@@ -25470,7 +25470,7 @@
       </c>
       <c r="AW30" s="11"/>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>39</v>
       </c>
@@ -25616,7 +25616,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -25813,7 +25813,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="33" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -26010,7 +26010,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="34" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -26207,7 +26207,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -26404,7 +26404,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="36" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -26601,11 +26601,11 @@
         <v>343.4</v>
       </c>
     </row>
-    <row r="37" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AL37" s="5"/>
       <c r="AM37" s="5"/>
     </row>
-    <row r="38" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -26802,7 +26802,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="39" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -26999,7 +26999,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="40" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -27196,7 +27196,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="41" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>37</v>
       </c>
@@ -27393,7 +27393,7 @@
         <v>16.399999999999977</v>
       </c>
     </row>
-    <row r="42" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -27590,10 +27590,10 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
     </row>
-    <row r="46" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
@@ -27613,10 +27613,10 @@
       <c r="X46" s="10"/>
       <c r="Y46" s="10"/>
     </row>
-    <row r="47" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
     </row>
-    <row r="48" spans="1:49" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>2</v>
       </c>
@@ -27638,7 +27638,7 @@
       <c r="X48" s="2"/>
       <c r="Y48" s="2"/>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>3</v>
       </c>
@@ -27660,7 +27660,7 @@
       <c r="X49" s="2"/>
       <c r="Y49" s="2"/>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>4</v>
       </c>
@@ -27682,7 +27682,7 @@
       <c r="X50" s="2"/>
       <c r="Y50" s="2"/>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>5</v>
       </c>
@@ -27704,7 +27704,7 @@
       <c r="X51" s="2"/>
       <c r="Y51" s="2"/>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>6</v>
       </c>
@@ -27726,10 +27726,10 @@
       <c r="X52" s="2"/>
       <c r="Y52" s="2"/>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>34</v>
       </c>
@@ -27751,7 +27751,7 @@
       <c r="X54" s="2"/>
       <c r="Y54" s="2"/>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>35</v>
       </c>
@@ -27773,7 +27773,7 @@
       <c r="X55" s="2"/>
       <c r="Y55" s="2"/>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>36</v>
       </c>
@@ -27795,7 +27795,7 @@
       <c r="X56" s="2"/>
       <c r="Y56" s="2"/>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>37</v>
       </c>
@@ -27817,7 +27817,7 @@
       <c r="X57" s="2"/>
       <c r="Y57" s="2"/>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>38</v>
       </c>
@@ -27839,17 +27839,29 @@
       <c r="X58" s="2"/>
       <c r="Y58" s="2"/>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="AV30:AW30"/>
+    <mergeCell ref="Z30:AA30"/>
+    <mergeCell ref="AB30:AC30"/>
+    <mergeCell ref="AD30:AE30"/>
+    <mergeCell ref="AF30:AG30"/>
+    <mergeCell ref="AH30:AI30"/>
+    <mergeCell ref="AJ30:AK30"/>
+    <mergeCell ref="AL30:AM30"/>
+    <mergeCell ref="AN30:AO30"/>
+    <mergeCell ref="AP30:AQ30"/>
+    <mergeCell ref="AR30:AS30"/>
+    <mergeCell ref="AT30:AU30"/>
     <mergeCell ref="X30:Y30"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="D30:E30"/>
@@ -27862,18 +27874,6 @@
     <mergeCell ref="R30:S30"/>
     <mergeCell ref="T30:U30"/>
     <mergeCell ref="V30:W30"/>
-    <mergeCell ref="AV30:AW30"/>
-    <mergeCell ref="Z30:AA30"/>
-    <mergeCell ref="AB30:AC30"/>
-    <mergeCell ref="AD30:AE30"/>
-    <mergeCell ref="AF30:AG30"/>
-    <mergeCell ref="AH30:AI30"/>
-    <mergeCell ref="AJ30:AK30"/>
-    <mergeCell ref="AL30:AM30"/>
-    <mergeCell ref="AN30:AO30"/>
-    <mergeCell ref="AP30:AQ30"/>
-    <mergeCell ref="AR30:AS30"/>
-    <mergeCell ref="AT30:AU30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>